<commit_message>
AutoCommit_12 апреля 2024 г. 9:04:19_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\2ОИБАС1322_ОпСис_\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\2ОИБАС1322\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>Лаб4</t>
-  </si>
-  <si>
-    <t>Сумма</t>
   </si>
 </sst>
 </file>
@@ -211,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -230,6 +227,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -534,13 +537,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S31" sqref="S31"/>
+      <selection pane="bottomRight" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -606,9 +609,6 @@
       <c r="E3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="R3" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="4" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
@@ -654,13 +654,7 @@
       <c r="P4" s="4">
         <v>5</v>
       </c>
-      <c r="R4">
-        <f>SUM(D4:P4)</f>
-        <v>55</v>
-      </c>
-      <c r="S4" s="7">
-        <v>5</v>
-      </c>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
@@ -677,13 +671,7 @@
       <c r="E5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="R5" s="6">
-        <f t="shared" ref="R5:R30" si="1">SUM(D5:P5)</f>
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>3</v>
-      </c>
+      <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
@@ -722,13 +710,7 @@
       <c r="P6" s="4">
         <v>5</v>
       </c>
-      <c r="R6" s="6">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="S6">
-        <v>5</v>
-      </c>
+      <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
@@ -745,13 +727,7 @@
       <c r="E7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="R7" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>3</v>
-      </c>
+      <c r="R7" s="6"/>
     </row>
     <row r="8" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
@@ -774,13 +750,7 @@
         <v>5</v>
       </c>
       <c r="M8" s="2"/>
-      <c r="R8" s="6">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="S8">
-        <v>3</v>
-      </c>
+      <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
@@ -812,13 +782,7 @@
         <v>5</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="R9" s="6">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="S9">
-        <v>5</v>
-      </c>
+      <c r="R9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
@@ -851,13 +815,7 @@
         <v>5</v>
       </c>
       <c r="M10" s="2"/>
-      <c r="R10" s="6">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="S10">
-        <v>5</v>
-      </c>
+      <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
@@ -890,13 +848,7 @@
         <v>5</v>
       </c>
       <c r="M11" s="2"/>
-      <c r="R11" s="6">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="S11">
-        <v>5</v>
-      </c>
+      <c r="R11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
@@ -917,13 +869,7 @@
         <v>5</v>
       </c>
       <c r="M12" s="2"/>
-      <c r="R12" s="6">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="S12">
-        <v>3</v>
-      </c>
+      <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
@@ -954,13 +900,7 @@
       <c r="M13" s="3">
         <v>5</v>
       </c>
-      <c r="R13" s="6">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="S13">
-        <v>5</v>
-      </c>
+      <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
@@ -991,13 +931,7 @@
         <v>5</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="R14" s="6">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="S14">
-        <v>4</v>
-      </c>
+      <c r="R14" s="6"/>
     </row>
     <row r="15" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
@@ -1014,13 +948,7 @@
       <c r="E15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="R15" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>3</v>
-      </c>
+      <c r="R15" s="6"/>
     </row>
     <row r="16" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
@@ -1039,13 +967,7 @@
       <c r="E16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="R16" s="6">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="S16">
-        <v>3</v>
-      </c>
+      <c r="R16" s="6"/>
     </row>
     <row r="17" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
@@ -1081,13 +1003,7 @@
         <v>5</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="R17" s="6">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="S17">
-        <v>5</v>
-      </c>
+      <c r="R17" s="6"/>
     </row>
     <row r="18" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
@@ -1125,13 +1041,7 @@
       <c r="P18" s="5">
         <v>5</v>
       </c>
-      <c r="R18" s="6">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="S18">
-        <v>5</v>
-      </c>
+      <c r="R18" s="6"/>
     </row>
     <row r="19" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
@@ -1175,13 +1085,7 @@
       <c r="P19" s="4">
         <v>5</v>
       </c>
-      <c r="R19" s="6">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="S19">
-        <v>5</v>
-      </c>
+      <c r="R19" s="6"/>
     </row>
     <row r="20" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
@@ -1205,13 +1109,7 @@
         <v>5</v>
       </c>
       <c r="M20" s="2"/>
-      <c r="R20" s="6">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="S20">
-        <v>3</v>
-      </c>
+      <c r="R20" s="6"/>
     </row>
     <row r="21" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
@@ -1252,13 +1150,7 @@
       <c r="P21" s="4">
         <v>5</v>
       </c>
-      <c r="R21" s="6">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="S21">
-        <v>5</v>
-      </c>
+      <c r="R21" s="6"/>
     </row>
     <row r="22" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
@@ -1288,13 +1180,7 @@
         <v>5</v>
       </c>
       <c r="M22" s="2"/>
-      <c r="R22" s="6">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="S22">
-        <v>4</v>
-      </c>
+      <c r="R22" s="6"/>
     </row>
     <row r="23" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
@@ -1317,13 +1203,7 @@
       <c r="M23" s="3">
         <v>5</v>
       </c>
-      <c r="R23" s="6">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="S23">
-        <v>3</v>
-      </c>
+      <c r="R23" s="6"/>
     </row>
     <row r="24" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
@@ -1342,13 +1222,7 @@
       <c r="E24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="R24" s="6">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="S24">
-        <v>3</v>
-      </c>
+      <c r="R24" s="6"/>
     </row>
     <row r="25" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
@@ -1378,13 +1252,7 @@
         <v>5</v>
       </c>
       <c r="M25" s="2"/>
-      <c r="R25" s="6">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="S25">
-        <v>3</v>
-      </c>
+      <c r="R25" s="6"/>
     </row>
     <row r="26" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
@@ -1430,13 +1298,7 @@
       <c r="P26" s="4">
         <v>5</v>
       </c>
-      <c r="R26" s="6">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="S26">
-        <v>5</v>
-      </c>
+      <c r="R26" s="6"/>
     </row>
     <row r="27" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
@@ -1477,13 +1339,7 @@
         <v>5</v>
       </c>
       <c r="M27" s="2"/>
-      <c r="R27" s="6">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="S27">
-        <v>5</v>
-      </c>
+      <c r="R27" s="6"/>
     </row>
     <row r="28" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
@@ -1513,13 +1369,7 @@
       <c r="P28" s="4">
         <v>5</v>
       </c>
-      <c r="R28" s="6">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="S28">
-        <v>4</v>
-      </c>
+      <c r="R28" s="6"/>
     </row>
     <row r="29" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
@@ -1540,13 +1390,7 @@
         <v>5</v>
       </c>
       <c r="M29" s="2"/>
-      <c r="R29" s="6">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="S29">
-        <v>3</v>
-      </c>
+      <c r="R29" s="6"/>
     </row>
     <row r="30" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
@@ -1584,233 +1428,325 @@
         <v>5</v>
       </c>
       <c r="M30" s="2"/>
-      <c r="R30" s="6">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="S30">
-        <v>5</v>
-      </c>
+      <c r="R30" s="6"/>
     </row>
     <row r="31" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="3">
-        <v>5</v>
-      </c>
-      <c r="E31" s="3">
-        <v>5</v>
-      </c>
-      <c r="F31" s="4">
-        <v>5</v>
-      </c>
-      <c r="G31" s="4">
-        <v>5</v>
-      </c>
-      <c r="H31" s="6"/>
-      <c r="I31" s="4">
-        <v>5</v>
-      </c>
-      <c r="J31" s="4">
-        <v>5</v>
-      </c>
-      <c r="K31" s="4">
-        <v>5</v>
-      </c>
-      <c r="L31" s="3">
-        <v>5</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="3">
-        <v>5</v>
-      </c>
-      <c r="E32" s="3">
-        <v>5</v>
-      </c>
-      <c r="F32" s="4">
-        <v>5</v>
-      </c>
-      <c r="G32" s="4">
-        <v>5</v>
-      </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="4">
-        <v>5</v>
-      </c>
-      <c r="J32" s="4">
-        <v>5</v>
-      </c>
-      <c r="K32" s="4">
-        <v>5</v>
-      </c>
-      <c r="L32" s="3">
-        <v>5</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-    </row>
-    <row r="33" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="3">
-        <v>5</v>
-      </c>
-      <c r="E33" s="3">
-        <v>5</v>
-      </c>
-      <c r="F33" s="4">
-        <v>5</v>
-      </c>
-      <c r="G33" s="4">
-        <v>5</v>
-      </c>
-      <c r="H33" s="6"/>
-      <c r="I33" s="4">
-        <v>5</v>
-      </c>
-      <c r="J33" s="4">
-        <v>5</v>
-      </c>
-      <c r="K33" s="4">
-        <v>5</v>
-      </c>
-      <c r="L33" s="3">
-        <v>5</v>
-      </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-    </row>
-    <row r="34" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="3">
-        <v>5</v>
-      </c>
-      <c r="E34" s="3">
-        <v>5</v>
-      </c>
-      <c r="F34" s="4">
-        <v>5</v>
-      </c>
-      <c r="G34" s="4">
-        <v>5</v>
-      </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="4">
-        <v>5</v>
-      </c>
-      <c r="J34" s="4">
-        <v>5</v>
-      </c>
-      <c r="K34" s="4">
-        <v>5</v>
-      </c>
-      <c r="L34" s="3">
-        <v>5</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-    </row>
-    <row r="35" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="3">
-        <v>5</v>
-      </c>
-      <c r="E35" s="3">
-        <v>5</v>
-      </c>
-      <c r="F35" s="4">
-        <v>5</v>
-      </c>
-      <c r="G35" s="4">
-        <v>5</v>
-      </c>
-      <c r="H35" s="6"/>
-      <c r="I35" s="4">
-        <v>5</v>
-      </c>
-      <c r="J35" s="4">
-        <v>5</v>
-      </c>
-      <c r="K35" s="4">
-        <v>5</v>
-      </c>
-      <c r="L35" s="3">
-        <v>5</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-    </row>
-    <row r="36" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="3">
-        <v>5</v>
-      </c>
-      <c r="E36" s="3">
-        <v>5</v>
-      </c>
-      <c r="F36" s="4">
-        <v>5</v>
-      </c>
-      <c r="G36" s="4">
-        <v>5</v>
-      </c>
-      <c r="H36" s="6"/>
-      <c r="I36" s="4">
-        <v>5</v>
-      </c>
-      <c r="J36" s="4">
-        <v>5</v>
-      </c>
-      <c r="K36" s="4">
-        <v>5</v>
-      </c>
-      <c r="L36" s="3">
-        <v>5</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-    </row>
-    <row r="37" spans="3:16" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+    </row>
+    <row r="33" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+    </row>
+    <row r="34" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+    </row>
+    <row r="35" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+    </row>
+    <row r="36" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+    </row>
+    <row r="37" spans="1:19" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="R4:R30">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 9:33:53_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
-  <si>
-    <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>Адеев Григорий</t>
   </si>
@@ -142,6 +139,27 @@
   </si>
   <si>
     <t>Лаб4</t>
+  </si>
+  <si>
+    <t>Лаб6</t>
+  </si>
+  <si>
+    <t>Лаб7</t>
+  </si>
+  <si>
+    <t>Лаб8</t>
+  </si>
+  <si>
+    <t>Лаб9</t>
+  </si>
+  <si>
+    <t>Лаб10</t>
+  </si>
+  <si>
+    <t>Лаб11</t>
+  </si>
+  <si>
+    <t>Тест</t>
   </si>
 </sst>
 </file>
@@ -181,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -204,11 +222,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -231,6 +260,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -537,13 +572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S45"/>
+  <dimension ref="A1:XFD44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P25" sqref="P25"/>
+      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -551,69 +586,135 @@
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
     <col min="2" max="2" width="21.453125" customWidth="1"/>
     <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="8" width="5.1796875" customWidth="1"/>
+    <col min="4" max="8" width="5.90625" customWidth="1"/>
+    <col min="9" max="11" width="5.81640625" customWidth="1"/>
+    <col min="12" max="20" width="5.6328125" customWidth="1"/>
+    <col min="21" max="22" width="6.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="1" t="s">
+    <row r="1" spans="1:23 16384:16384" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="S1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="XFD1" s="1"/>
+    </row>
+    <row r="2" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <f>IF(B3=C3,A2+1,"-----------------")</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5</v>
+      </c>
+      <c r="I3" s="4">
+        <v>5</v>
+      </c>
+      <c r="J3" s="9">
+        <v>5</v>
+      </c>
+      <c r="M3" s="3">
+        <v>5</v>
+      </c>
+      <c r="N3" s="3">
+        <v>5</v>
+      </c>
+      <c r="O3" s="4">
+        <v>5</v>
+      </c>
+      <c r="P3" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>5</v>
+      </c>
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
-        <f>IF(B4=C4,A3+1,"-----------------")</f>
-        <v>1</v>
+        <f t="shared" ref="A4:A29" si="0">IF(B4=C4,A3+1,"-----------------")</f>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -621,45 +722,19 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3">
-        <v>5</v>
-      </c>
-      <c r="F4" s="4">
-        <v>5</v>
-      </c>
-      <c r="G4" s="4">
-        <v>5</v>
-      </c>
-      <c r="I4" s="4">
-        <v>5</v>
-      </c>
-      <c r="J4" s="9">
-        <v>5</v>
-      </c>
-      <c r="L4" s="3">
-        <v>5</v>
-      </c>
-      <c r="M4" s="3">
-        <v>5</v>
-      </c>
-      <c r="N4" s="4">
-        <v>5</v>
-      </c>
-      <c r="O4" s="4">
-        <v>5</v>
-      </c>
-      <c r="P4" s="4">
-        <v>5</v>
-      </c>
-      <c r="S4" s="7"/>
-    </row>
-    <row r="5" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="S4" s="6"/>
+    </row>
+    <row r="5" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
-        <f t="shared" ref="A5:A30" si="0">IF(B5=C5,A4+1,"-----------------")</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -668,15 +743,45 @@
         <v>2</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4">
+        <v>5</v>
+      </c>
+      <c r="I5" s="4">
+        <v>5</v>
+      </c>
+      <c r="J5" s="4">
+        <v>5</v>
+      </c>
+      <c r="K5" s="4">
+        <v>5</v>
+      </c>
+      <c r="L5" s="8">
+        <v>5</v>
+      </c>
       <c r="M5" s="2"/>
-      <c r="R5" s="6"/>
-    </row>
-    <row r="6" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -685,37 +790,15 @@
         <v>3</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="3">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4">
-        <v>5</v>
-      </c>
-      <c r="G6" s="4">
-        <v>5</v>
-      </c>
-      <c r="I6" s="4">
-        <v>5</v>
-      </c>
-      <c r="J6" s="4">
-        <v>5</v>
-      </c>
-      <c r="K6" s="4">
-        <v>5</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="3">
-        <v>5</v>
-      </c>
-      <c r="P6" s="4">
-        <v>5</v>
-      </c>
-      <c r="R6" s="6"/>
-    </row>
-    <row r="7" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="S6" s="6"/>
+    </row>
+    <row r="7" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -723,16 +806,25 @@
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="R7" s="6"/>
-    </row>
-    <row r="8" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="M7" s="3">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -746,16 +838,25 @@
       <c r="E8" s="3">
         <v>5</v>
       </c>
-      <c r="L8" s="3">
-        <v>5</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="R8" s="6"/>
-    </row>
-    <row r="9" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="4">
+        <v>5</v>
+      </c>
+      <c r="I8" s="4">
+        <v>5</v>
+      </c>
+      <c r="J8" s="4">
+        <v>5</v>
+      </c>
+      <c r="M8" s="3">
+        <v>5</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -763,12 +864,13 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3">
-        <v>5</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="3">
         <v>5</v>
       </c>
+      <c r="F9" s="4">
+        <v>5</v>
+      </c>
       <c r="G9" s="4">
         <v>5</v>
       </c>
@@ -778,16 +880,21 @@
       <c r="J9" s="4">
         <v>5</v>
       </c>
-      <c r="L9" s="3">
-        <v>5</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="R9" s="6"/>
-    </row>
-    <row r="10" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="8">
+        <v>5</v>
+      </c>
+      <c r="M9" s="3">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="S9" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -811,16 +918,16 @@
       <c r="J10" s="4">
         <v>5</v>
       </c>
-      <c r="L10" s="3">
-        <v>5</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="R10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="3">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -828,32 +935,20 @@
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3">
-        <v>5</v>
-      </c>
-      <c r="F11" s="4">
-        <v>5</v>
-      </c>
-      <c r="G11" s="4">
-        <v>5</v>
-      </c>
-      <c r="I11" s="4">
-        <v>5</v>
-      </c>
-      <c r="J11" s="4">
-        <v>5</v>
-      </c>
-      <c r="L11" s="3">
-        <v>5</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="R11" s="6"/>
-    </row>
-    <row r="12" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="M11" s="3">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -864,17 +959,27 @@
       <c r="D12" s="3">
         <v>5</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="L12" s="3">
-        <v>5</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="R12" s="6"/>
-    </row>
-    <row r="13" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5</v>
+      </c>
+      <c r="G12" s="4">
+        <v>5</v>
+      </c>
+      <c r="M12" s="3">
+        <v>5</v>
+      </c>
+      <c r="N12" s="3">
+        <v>5</v>
+      </c>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -882,30 +987,30 @@
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="3">
-        <v>5</v>
-      </c>
-      <c r="E13" s="3">
-        <v>5</v>
-      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="4">
         <v>5</v>
       </c>
       <c r="G13" s="4">
         <v>5</v>
       </c>
-      <c r="L13" s="3">
+      <c r="I13" s="8">
+        <v>5</v>
+      </c>
+      <c r="J13" s="8">
         <v>5</v>
       </c>
       <c r="M13" s="3">
         <v>5</v>
       </c>
-      <c r="R13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="2"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -915,28 +1020,14 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="4">
-        <v>5</v>
-      </c>
-      <c r="G14" s="4">
-        <v>5</v>
-      </c>
-      <c r="I14" s="8">
-        <v>5</v>
-      </c>
-      <c r="J14" s="8">
-        <v>5</v>
-      </c>
-      <c r="L14" s="3">
-        <v>5</v>
-      </c>
       <c r="M14" s="2"/>
-      <c r="R14" s="6"/>
-    </row>
-    <row r="15" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="2"/>
+      <c r="S14" s="6"/>
+    </row>
+    <row r="15" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -944,16 +1035,18 @@
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="3">
+        <v>5</v>
+      </c>
       <c r="E15" s="2"/>
-      <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="R15" s="6"/>
-    </row>
-    <row r="16" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N15" s="2"/>
+      <c r="S15" s="6"/>
+    </row>
+    <row r="16" spans="1:23 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -961,18 +1054,44 @@
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="3">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="R16" s="6"/>
-    </row>
-    <row r="17" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="2"/>
+      <c r="E16" s="3">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>5</v>
+      </c>
+      <c r="G16" s="4">
+        <v>5</v>
+      </c>
+      <c r="I16" s="4">
+        <v>5</v>
+      </c>
+      <c r="J16" s="4">
+        <v>5</v>
+      </c>
+      <c r="K16" s="4">
+        <v>5</v>
+      </c>
+      <c r="M16" s="3">
+        <v>5</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="R16">
+        <v>5</v>
+      </c>
+      <c r="S16" s="6"/>
+      <c r="U16">
+        <v>5</v>
+      </c>
+      <c r="W16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -996,19 +1115,29 @@
       <c r="J17" s="4">
         <v>5</v>
       </c>
-      <c r="K17" s="4">
-        <v>5</v>
-      </c>
-      <c r="L17" s="3">
-        <v>5</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="R17" s="6"/>
-    </row>
-    <row r="18" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="3">
+        <v>5</v>
+      </c>
+      <c r="N17" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>5</v>
+      </c>
+      <c r="R17" s="12">
+        <v>5</v>
+      </c>
+      <c r="S17" s="6">
+        <v>5</v>
+      </c>
+      <c r="W17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
@@ -1026,27 +1155,33 @@
       <c r="G18" s="4">
         <v>5</v>
       </c>
+      <c r="H18" s="4">
+        <v>5</v>
+      </c>
       <c r="I18" s="4">
         <v>5</v>
       </c>
       <c r="J18" s="4">
         <v>5</v>
       </c>
-      <c r="L18" s="3">
+      <c r="K18" s="4">
         <v>5</v>
       </c>
       <c r="M18" s="3">
         <v>5</v>
       </c>
-      <c r="P18" s="5">
-        <v>5</v>
-      </c>
-      <c r="R18" s="6"/>
-    </row>
-    <row r="19" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>5</v>
+      </c>
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
@@ -1061,36 +1196,16 @@
       <c r="F19" s="4">
         <v>5</v>
       </c>
-      <c r="G19" s="4">
-        <v>5</v>
-      </c>
-      <c r="H19" s="4">
-        <v>5</v>
-      </c>
-      <c r="I19" s="4">
-        <v>5</v>
-      </c>
-      <c r="J19" s="4">
-        <v>5</v>
-      </c>
-      <c r="K19" s="4">
-        <v>5</v>
-      </c>
-      <c r="L19" s="3">
-        <v>5</v>
-      </c>
       <c r="M19" s="3">
         <v>5</v>
       </c>
-      <c r="P19" s="4">
-        <v>5</v>
-      </c>
-      <c r="R19" s="6"/>
-    </row>
-    <row r="20" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="2"/>
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
@@ -1099,22 +1214,42 @@
         <v>17</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>5</v>
       </c>
       <c r="F20" s="4">
         <v>5</v>
       </c>
-      <c r="L20" s="3">
-        <v>5</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="R20" s="6"/>
-    </row>
-    <row r="21" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="8">
+        <v>5</v>
+      </c>
+      <c r="I20" s="8">
+        <v>5</v>
+      </c>
+      <c r="J20" s="4">
+        <v>5</v>
+      </c>
+      <c r="K20" s="4">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20" s="3">
+        <v>5</v>
+      </c>
+      <c r="N20" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>5</v>
+      </c>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -1122,40 +1257,32 @@
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2">
-        <v>5</v>
-      </c>
+      <c r="D21" s="3">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="4">
         <v>5</v>
       </c>
-      <c r="G21" s="8">
-        <v>5</v>
-      </c>
-      <c r="I21" s="8">
-        <v>5</v>
-      </c>
-      <c r="J21" s="4">
+      <c r="G21" s="4">
         <v>5</v>
       </c>
       <c r="K21" s="4">
         <v>5</v>
       </c>
-      <c r="L21" s="3">
-        <v>5</v>
-      </c>
-      <c r="M21" s="2">
-        <v>5</v>
-      </c>
-      <c r="P21" s="4">
-        <v>5</v>
-      </c>
-      <c r="R21" s="6"/>
-    </row>
-    <row r="22" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>5</v>
+      </c>
+      <c r="M21" s="3">
+        <v>5</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -1167,25 +1294,18 @@
         <v>5</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="4">
-        <v>5</v>
-      </c>
-      <c r="G22" s="4">
-        <v>5</v>
-      </c>
-      <c r="K22" s="4">
-        <v>5</v>
-      </c>
-      <c r="L22" s="3">
-        <v>5</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="R22" s="6"/>
-    </row>
-    <row r="23" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="3">
+        <v>5</v>
+      </c>
+      <c r="N22" s="3">
+        <v>5</v>
+      </c>
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
@@ -1197,18 +1317,14 @@
         <v>5</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="L23" s="3">
-        <v>5</v>
-      </c>
-      <c r="M23" s="3">
-        <v>5</v>
-      </c>
-      <c r="R23" s="6"/>
-    </row>
-    <row r="24" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>21</v>
@@ -1216,18 +1332,32 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="3">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="R24" s="6"/>
-    </row>
-    <row r="25" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="2"/>
+      <c r="E24" s="3">
+        <v>5</v>
+      </c>
+      <c r="F24" s="4">
+        <v>4</v>
+      </c>
+      <c r="I24" s="4">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="M24" s="3">
+        <v>5</v>
+      </c>
+      <c r="N24" s="2"/>
+      <c r="R24">
+        <v>5</v>
+      </c>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
@@ -1235,29 +1365,48 @@
       <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="3">
+        <v>5</v>
+      </c>
       <c r="E25" s="3">
         <v>5</v>
       </c>
       <c r="F25" s="4">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G25" s="4">
+        <v>5</v>
+      </c>
+      <c r="H25" s="4">
+        <v>5</v>
       </c>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25">
-        <v>5</v>
-      </c>
-      <c r="L25" s="3">
-        <v>5</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="R25" s="6"/>
-    </row>
-    <row r="26" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="4">
+        <v>5</v>
+      </c>
+      <c r="K25" s="4">
+        <v>5</v>
+      </c>
+      <c r="L25" s="8">
+        <v>5</v>
+      </c>
+      <c r="M25" s="3">
+        <v>5</v>
+      </c>
+      <c r="N25" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>5</v>
+      </c>
+      <c r="S25" s="6"/>
+    </row>
+    <row r="26" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
@@ -1289,21 +1438,16 @@
       <c r="K26" s="4">
         <v>5</v>
       </c>
-      <c r="L26" s="3">
-        <v>5</v>
-      </c>
       <c r="M26" s="3">
         <v>5</v>
       </c>
-      <c r="P26" s="4">
-        <v>5</v>
-      </c>
-      <c r="R26" s="6"/>
-    </row>
-    <row r="27" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="2"/>
+      <c r="S26" s="6"/>
+    </row>
+    <row r="27" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -1311,40 +1455,29 @@
       <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="3">
-        <v>5</v>
-      </c>
-      <c r="E27" s="3">
-        <v>5</v>
-      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="4">
         <v>5</v>
       </c>
       <c r="G27" s="4">
         <v>5</v>
       </c>
-      <c r="H27" s="4">
-        <v>5</v>
-      </c>
-      <c r="I27" s="4">
-        <v>5</v>
-      </c>
-      <c r="J27" s="4">
-        <v>5</v>
-      </c>
-      <c r="K27" s="4">
-        <v>5</v>
-      </c>
-      <c r="L27" s="3">
-        <v>5</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="R27" s="6"/>
-    </row>
-    <row r="28" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="3">
+        <v>5</v>
+      </c>
+      <c r="N27" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>5</v>
+      </c>
+      <c r="S27" s="6"/>
+    </row>
+    <row r="28" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
@@ -1352,29 +1485,20 @@
       <c r="C28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="3">
+        <v>5</v>
+      </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="4">
-        <v>5</v>
-      </c>
-      <c r="G28" s="4">
-        <v>5</v>
-      </c>
-      <c r="L28" s="3">
-        <v>5</v>
-      </c>
       <c r="M28" s="3">
         <v>5</v>
       </c>
-      <c r="P28" s="4">
-        <v>5</v>
-      </c>
-      <c r="R28" s="6"/>
-    </row>
-    <row r="29" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="2"/>
+      <c r="S28" s="6"/>
+    </row>
+    <row r="29" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
@@ -1385,52 +1509,55 @@
       <c r="D29" s="3">
         <v>5</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="L29" s="3">
-        <v>5</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="R29" s="6"/>
-    </row>
-    <row r="30" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="3">
-        <v>5</v>
-      </c>
-      <c r="E30" s="3">
-        <v>5</v>
-      </c>
-      <c r="F30" s="4">
-        <v>5</v>
-      </c>
-      <c r="G30" s="4">
-        <v>5</v>
-      </c>
-      <c r="I30" s="4">
-        <v>5</v>
-      </c>
-      <c r="J30" s="4">
-        <v>5</v>
-      </c>
-      <c r="K30" s="4">
-        <v>5</v>
-      </c>
-      <c r="L30" s="3">
-        <v>5</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="R30" s="6"/>
-    </row>
-    <row r="31" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="3">
+        <v>5</v>
+      </c>
+      <c r="F29" s="4">
+        <v>5</v>
+      </c>
+      <c r="G29" s="4">
+        <v>5</v>
+      </c>
+      <c r="I29" s="4">
+        <v>5</v>
+      </c>
+      <c r="J29" s="4">
+        <v>5</v>
+      </c>
+      <c r="K29" s="4">
+        <v>5</v>
+      </c>
+      <c r="M29" s="3">
+        <v>5</v>
+      </c>
+      <c r="N29" s="2"/>
+      <c r="R29">
+        <v>5</v>
+      </c>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+    </row>
+    <row r="31" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="10"/>
@@ -1442,16 +1569,16 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
-      <c r="L31" s="11"/>
       <c r="M31" s="11"/>
-      <c r="N31" s="8"/>
+      <c r="N31" s="11"/>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
-    </row>
-    <row r="32" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T31" s="8"/>
+    </row>
+    <row r="32" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="10"/>
@@ -1463,16 +1590,16 @@
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
-      <c r="L32" s="11"/>
       <c r="M32" s="11"/>
-      <c r="N32" s="8"/>
+      <c r="N32" s="11"/>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
-    </row>
-    <row r="33" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T32" s="8"/>
+    </row>
+    <row r="33" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="10"/>
@@ -1484,16 +1611,16 @@
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="11"/>
       <c r="M33" s="11"/>
-      <c r="N33" s="8"/>
+      <c r="N33" s="11"/>
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
-    </row>
-    <row r="34" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T33" s="8"/>
+    </row>
+    <row r="34" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="10"/>
@@ -1505,16 +1632,16 @@
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="11"/>
       <c r="M34" s="11"/>
-      <c r="N34" s="8"/>
+      <c r="N34" s="11"/>
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
-    </row>
-    <row r="35" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T34" s="8"/>
+    </row>
+    <row r="35" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="10"/>
@@ -1526,29 +1653,29 @@
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="11"/>
       <c r="M35" s="11"/>
-      <c r="N35" s="8"/>
+      <c r="N35" s="11"/>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
-    </row>
-    <row r="36" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T35" s="8"/>
+    </row>
+    <row r="36" spans="1:20" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
       <c r="P36" s="8"/>
@@ -1556,7 +1683,7 @@
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
     </row>
-    <row r="37" spans="1:19" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -1577,7 +1704,7 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1598,7 +1725,7 @@
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1619,7 +1746,7 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1640,7 +1767,7 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1661,7 +1788,7 @@
       <c r="R41" s="8"/>
       <c r="S41" s="8"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1682,7 +1809,7 @@
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -1703,7 +1830,7 @@
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -1724,27 +1851,6 @@
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="8"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AutoCommit_22 июня 2024 г. 16:40:40_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>Адеев Григорий</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>его нет</t>
+  </si>
+  <si>
+    <t>ковалев</t>
+  </si>
+  <si>
+    <t>-----------------</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -280,6 +286,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -590,7 +597,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Z14" sqref="Z14"/>
+      <selection pane="bottomRight" activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -682,6 +689,9 @@
       <c r="E2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
+      <c r="AA2" s="15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
@@ -730,6 +740,9 @@
       <c r="T3" s="7"/>
       <c r="Z3">
         <v>11</v>
+      </c>
+      <c r="AA3">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -754,6 +767,9 @@
       <c r="Z4">
         <v>13</v>
       </c>
+      <c r="AA4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
@@ -803,6 +819,9 @@
       </c>
       <c r="Z5">
         <v>28</v>
+      </c>
+      <c r="AA5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -824,6 +843,9 @@
       <c r="Z6">
         <v>9</v>
       </c>
+      <c r="AA6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
@@ -852,6 +874,9 @@
       <c r="S7" s="6"/>
       <c r="Z7">
         <v>14</v>
+      </c>
+      <c r="AA7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -888,6 +913,9 @@
       <c r="Z8">
         <v>1</v>
       </c>
+      <c r="AA8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
@@ -928,6 +956,9 @@
       </c>
       <c r="Z9">
         <v>10</v>
+      </c>
+      <c r="AA9">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -965,6 +996,9 @@
       <c r="Z10">
         <v>19</v>
       </c>
+      <c r="AA10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
@@ -989,6 +1023,9 @@
       <c r="Z11">
         <v>8</v>
       </c>
+      <c r="AA11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
@@ -1022,6 +1059,9 @@
       <c r="S12" s="6"/>
       <c r="Z12">
         <v>20</v>
+      </c>
+      <c r="AA12">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1056,6 +1096,9 @@
       <c r="S13" s="6"/>
       <c r="Z13">
         <v>25</v>
+      </c>
+      <c r="AA13">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1074,6 +1117,9 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="S14" s="6"/>
+      <c r="Z14" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
@@ -1096,6 +1142,9 @@
       <c r="Z15">
         <v>16</v>
       </c>
+      <c r="AA15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
@@ -1148,7 +1197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1196,8 +1245,11 @@
       <c r="Z17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1243,8 +1295,11 @@
       <c r="Z18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1270,8 +1325,11 @@
       <c r="Z19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1318,7 +1376,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1353,8 +1411,11 @@
       <c r="Z21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1379,8 +1440,11 @@
       <c r="Z22">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1401,8 +1465,11 @@
       <c r="Z23">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1437,8 +1504,11 @@
       <c r="Z24">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1489,8 +1559,11 @@
       <c r="Z25">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1533,8 +1606,11 @@
       <c r="Z26">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1566,8 +1642,11 @@
       <c r="Z27">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1590,8 +1669,11 @@
       <c r="Z28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1634,10 +1716,15 @@
       <c r="Z29">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
+      <c r="B30" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
@@ -1655,8 +1742,14 @@
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
       <c r="T30" s="8"/>
-    </row>
-    <row r="31" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z30">
+        <v>26</v>
+      </c>
+      <c r="AA30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="10"/>
@@ -1677,7 +1770,7 @@
       <c r="S31" s="8"/>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="10"/>

</xml_diff>

<commit_message>
AutoCommit_22 июня 2024 г. 16:50:26_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -597,7 +597,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AA23" sqref="AA23"/>
+      <selection pane="bottomRight" activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1296,7 @@
         <v>2</v>
       </c>
       <c r="AA18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_28 июня 2024 г. 22:11:19_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>Адеев Григорий</t>
   </si>
@@ -102,63 +102,6 @@
     <t>Чередова Елизавета</t>
   </si>
   <si>
-    <t>Лаб1</t>
-  </si>
-  <si>
-    <t>Инд2</t>
-  </si>
-  <si>
-    <t>Инд1</t>
-  </si>
-  <si>
-    <t>Лаб2</t>
-  </si>
-  <si>
-    <t>Инд3</t>
-  </si>
-  <si>
-    <t>Инд4</t>
-  </si>
-  <si>
-    <t>Лаб5</t>
-  </si>
-  <si>
-    <t>Инд5</t>
-  </si>
-  <si>
-    <t>Инд6</t>
-  </si>
-  <si>
-    <t>Инд7</t>
-  </si>
-  <si>
-    <t>Инд8</t>
-  </si>
-  <si>
-    <t>Лаб3</t>
-  </si>
-  <si>
-    <t>Лаб4</t>
-  </si>
-  <si>
-    <t>Лаб6</t>
-  </si>
-  <si>
-    <t>Лаб7</t>
-  </si>
-  <si>
-    <t>Лаб8</t>
-  </si>
-  <si>
-    <t>Лаб9</t>
-  </si>
-  <si>
-    <t>Лаб10</t>
-  </si>
-  <si>
-    <t>Лаб11</t>
-  </si>
-  <si>
     <t>Тест</t>
   </si>
   <si>
@@ -175,6 +118,60 @@
   </si>
   <si>
     <t>-----------------</t>
+  </si>
+  <si>
+    <t>И 1</t>
+  </si>
+  <si>
+    <t>И 2</t>
+  </si>
+  <si>
+    <t>И 3</t>
+  </si>
+  <si>
+    <t>И 4</t>
+  </si>
+  <si>
+    <t>И 5</t>
+  </si>
+  <si>
+    <t>И 6</t>
+  </si>
+  <si>
+    <t>И 7</t>
+  </si>
+  <si>
+    <t>И 8</t>
+  </si>
+  <si>
+    <t>Л 1</t>
+  </si>
+  <si>
+    <t>Л 2</t>
+  </si>
+  <si>
+    <t>Л 5</t>
+  </si>
+  <si>
+    <t>Л 6</t>
+  </si>
+  <si>
+    <t>Л 7</t>
+  </si>
+  <si>
+    <t>Л 8</t>
+  </si>
+  <si>
+    <t>Л 9</t>
+  </si>
+  <si>
+    <t>Л 10</t>
+  </si>
+  <si>
+    <t>Л 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Л 3-4 </t>
   </si>
 </sst>
 </file>
@@ -591,13 +588,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD44"/>
+  <dimension ref="A1:XFC44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AB18" sqref="AB18"/>
+      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -605,82 +602,81 @@
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
     <col min="2" max="2" width="21.453125" customWidth="1"/>
     <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="8" width="5.90625" customWidth="1"/>
-    <col min="9" max="11" width="5.81640625" customWidth="1"/>
-    <col min="12" max="20" width="5.6328125" customWidth="1"/>
-    <col min="21" max="22" width="6.6328125" customWidth="1"/>
+    <col min="4" max="11" width="3" customWidth="1"/>
+    <col min="12" max="12" width="5.6328125" customWidth="1"/>
+    <col min="13" max="14" width="2.6328125" customWidth="1"/>
+    <col min="15" max="15" width="5.1796875" customWidth="1"/>
+    <col min="16" max="20" width="2.6328125" customWidth="1"/>
+    <col min="21" max="22" width="2.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27 16384:16384" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26 16383:16383" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA1" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="XFD1" s="1"/>
-    </row>
-    <row r="2" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="XFC1" s="1"/>
+    </row>
+    <row r="2" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>0</f>
         <v>0</v>
@@ -689,11 +685,11 @@
       <c r="E2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="AA2" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z2" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f>IF(B3=C3,A2+1,"-----------------")</f>
         <v>1</v>
@@ -734,18 +730,15 @@
       <c r="P3" s="4">
         <v>5</v>
       </c>
-      <c r="Q3" s="4">
-        <v>5</v>
-      </c>
-      <c r="T3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="Y3">
+        <v>11</v>
+      </c>
       <c r="Z3">
-        <v>11</v>
-      </c>
-      <c r="AA3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A29" si="0">IF(B4=C4,A3+1,"-----------------")</f>
         <v>2</v>
@@ -763,15 +756,26 @@
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="S4" s="6"/>
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4" s="6">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="Y4">
+        <v>13</v>
+      </c>
       <c r="Z4">
-        <v>13</v>
-      </c>
-      <c r="AA4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -808,23 +812,23 @@
       <c r="N5" s="3">
         <v>5</v>
       </c>
-      <c r="Q5" s="4">
-        <v>5</v>
-      </c>
-      <c r="R5">
-        <v>5</v>
-      </c>
-      <c r="S5" s="6">
-        <v>5</v>
+      <c r="P5" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5" s="6">
+        <v>5</v>
+      </c>
+      <c r="Y5">
+        <v>28</v>
       </c>
       <c r="Z5">
-        <v>28</v>
-      </c>
-      <c r="AA5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -839,15 +843,15 @@
       <c r="E6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="S6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="Y6">
+        <v>9</v>
+      </c>
       <c r="Z6">
-        <v>9</v>
-      </c>
-      <c r="AA6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -868,18 +872,21 @@
         <v>5</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="R7">
-        <v>5</v>
-      </c>
-      <c r="S7" s="6"/>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7" s="6"/>
+      <c r="Y7">
+        <v>14</v>
+      </c>
       <c r="Z7">
-        <v>14</v>
-      </c>
-      <c r="AA7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -909,15 +916,15 @@
         <v>5</v>
       </c>
       <c r="N8" s="2"/>
-      <c r="S8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="Y8">
+        <v>1</v>
+      </c>
       <c r="Z8">
-        <v>1</v>
-      </c>
-      <c r="AA8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -951,17 +958,26 @@
         <v>5</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="S9" s="6">
-        <v>5</v>
+      <c r="R9" s="6">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>5</v>
+      </c>
+      <c r="T9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="Y9">
+        <v>10</v>
       </c>
       <c r="Z9">
-        <v>10</v>
-      </c>
-      <c r="AA9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -992,15 +1008,15 @@
         <v>5</v>
       </c>
       <c r="N10" s="2"/>
-      <c r="S10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="Y10">
+        <v>19</v>
+      </c>
       <c r="Z10">
-        <v>19</v>
-      </c>
-      <c r="AA10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1019,15 +1035,15 @@
         <v>5</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="S11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="Y11">
+        <v>8</v>
+      </c>
       <c r="Z11">
-        <v>8</v>
-      </c>
-      <c r="AA11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1056,15 +1072,15 @@
       <c r="N12" s="3">
         <v>5</v>
       </c>
-      <c r="S12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="Y12">
+        <v>20</v>
+      </c>
       <c r="Z12">
-        <v>20</v>
-      </c>
-      <c r="AA12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1093,15 +1109,15 @@
         <v>5</v>
       </c>
       <c r="N13" s="2"/>
-      <c r="S13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="Y13">
+        <v>25</v>
+      </c>
       <c r="Z13">
-        <v>25</v>
-      </c>
-      <c r="AA13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1116,12 +1132,12 @@
       <c r="E14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="S14" s="6"/>
-      <c r="Z14" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R14" s="6"/>
+      <c r="Y14" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1138,15 +1154,15 @@
       <c r="E15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="S15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="Y15">
+        <v>16</v>
+      </c>
       <c r="Z15">
-        <v>16</v>
-      </c>
-      <c r="AA15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1180,24 +1196,35 @@
         <v>5</v>
       </c>
       <c r="N16" s="2"/>
-      <c r="R16">
-        <v>5</v>
-      </c>
-      <c r="S16" s="6"/>
-      <c r="U16">
-        <v>5</v>
-      </c>
-      <c r="W16">
-        <v>5</v>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16" s="6">
+        <v>5</v>
+      </c>
+      <c r="S16">
+        <v>5</v>
+      </c>
+      <c r="T16">
+        <v>5</v>
+      </c>
+      <c r="V16">
+        <v>5</v>
+      </c>
+      <c r="Y16">
+        <v>22</v>
       </c>
       <c r="Z16">
-        <v>22</v>
-      </c>
-      <c r="AA16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1230,26 +1257,26 @@
       <c r="N17" s="3">
         <v>5</v>
       </c>
-      <c r="Q17" s="5">
-        <v>5</v>
-      </c>
-      <c r="R17" s="12">
-        <v>5</v>
-      </c>
-      <c r="S17" s="6">
-        <v>5</v>
-      </c>
-      <c r="W17">
-        <v>5</v>
+      <c r="P17" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="12">
+        <v>5</v>
+      </c>
+      <c r="R17" s="6">
+        <v>5</v>
+      </c>
+      <c r="V17">
+        <v>5</v>
+      </c>
+      <c r="Y17">
+        <v>9</v>
       </c>
       <c r="Z17">
-        <v>9</v>
-      </c>
-      <c r="AA17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1288,18 +1315,18 @@
       <c r="N18" s="3">
         <v>5</v>
       </c>
-      <c r="Q18" s="4">
-        <v>5</v>
-      </c>
-      <c r="S18" s="6"/>
+      <c r="P18" s="4">
+        <v>5</v>
+      </c>
+      <c r="R18" s="6"/>
+      <c r="Y18">
+        <v>2</v>
+      </c>
       <c r="Z18">
-        <v>2</v>
-      </c>
-      <c r="AA18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1321,15 +1348,15 @@
         <v>5</v>
       </c>
       <c r="N19" s="2"/>
-      <c r="S19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="Y19">
+        <v>17</v>
+      </c>
       <c r="Z19">
-        <v>17</v>
-      </c>
-      <c r="AA19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1368,15 +1395,15 @@
       <c r="N20" s="2">
         <v>5</v>
       </c>
-      <c r="Q20" s="4">
-        <v>5</v>
-      </c>
-      <c r="S20" s="6"/>
-      <c r="Z20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P20" s="4">
+        <v>5</v>
+      </c>
+      <c r="R20" s="6"/>
+      <c r="Y20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1407,15 +1434,15 @@
         <v>5</v>
       </c>
       <c r="N21" s="2"/>
-      <c r="S21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="Y21">
+        <v>3</v>
+      </c>
       <c r="Z21">
-        <v>3</v>
-      </c>
-      <c r="AA21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1436,15 +1463,15 @@
       <c r="N22" s="3">
         <v>5</v>
       </c>
-      <c r="S22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="Y22">
+        <v>12</v>
+      </c>
       <c r="Z22">
-        <v>12</v>
-      </c>
-      <c r="AA22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1461,15 +1488,15 @@
       <c r="E23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
-      <c r="S23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="Y23">
+        <v>21</v>
+      </c>
       <c r="Z23">
-        <v>21</v>
-      </c>
-      <c r="AA23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1497,18 +1524,26 @@
         <v>5</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="R24">
-        <v>5</v>
-      </c>
-      <c r="S24" s="6"/>
+      <c r="O24">
+        <v>5</v>
+      </c>
+      <c r="P24">
+        <v>5</v>
+      </c>
+      <c r="Q24">
+        <v>5</v>
+      </c>
+      <c r="R24" s="6">
+        <v>5</v>
+      </c>
+      <c r="Y24">
+        <v>18</v>
+      </c>
       <c r="Z24">
-        <v>18</v>
-      </c>
-      <c r="AA24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1552,18 +1587,29 @@
       <c r="N25" s="3">
         <v>5</v>
       </c>
-      <c r="Q25" s="4">
-        <v>5</v>
-      </c>
-      <c r="S25" s="6"/>
+      <c r="P25" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q25">
+        <v>5</v>
+      </c>
+      <c r="R25" s="6">
+        <v>5</v>
+      </c>
+      <c r="S25">
+        <v>5</v>
+      </c>
+      <c r="T25">
+        <v>5</v>
+      </c>
+      <c r="Y25">
+        <v>27</v>
+      </c>
       <c r="Z25">
-        <v>27</v>
-      </c>
-      <c r="AA25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1602,15 +1648,38 @@
         <v>5</v>
       </c>
       <c r="N26" s="2"/>
-      <c r="S26" s="6"/>
+      <c r="O26">
+        <v>5</v>
+      </c>
+      <c r="P26">
+        <v>5</v>
+      </c>
+      <c r="Q26">
+        <v>5</v>
+      </c>
+      <c r="R26" s="6">
+        <v>5</v>
+      </c>
+      <c r="S26">
+        <v>5</v>
+      </c>
+      <c r="T26">
+        <v>5</v>
+      </c>
+      <c r="U26">
+        <v>5</v>
+      </c>
+      <c r="V26">
+        <v>5</v>
+      </c>
+      <c r="Y26">
+        <v>22</v>
+      </c>
       <c r="Z26">
-        <v>22</v>
-      </c>
-      <c r="AA26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1635,18 +1704,18 @@
       <c r="N27" s="3">
         <v>5</v>
       </c>
-      <c r="Q27" s="4">
-        <v>5</v>
-      </c>
-      <c r="S27" s="6"/>
+      <c r="P27" s="4">
+        <v>5</v>
+      </c>
+      <c r="R27" s="6"/>
+      <c r="Y27">
+        <v>6</v>
+      </c>
       <c r="Z27">
-        <v>6</v>
-      </c>
-      <c r="AA27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1665,15 +1734,15 @@
         <v>5</v>
       </c>
       <c r="N28" s="2"/>
-      <c r="S28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="Y28">
+        <v>5</v>
+      </c>
       <c r="Z28">
-        <v>5</v>
-      </c>
-      <c r="AA28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1709,21 +1778,21 @@
         <v>5</v>
       </c>
       <c r="N29" s="2"/>
-      <c r="R29">
-        <v>5</v>
-      </c>
-      <c r="S29" s="6"/>
+      <c r="Q29">
+        <v>5</v>
+      </c>
+      <c r="R29" s="6"/>
+      <c r="Y29">
+        <v>15</v>
+      </c>
       <c r="Z29">
-        <v>15</v>
-      </c>
-      <c r="AA29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
@@ -1741,15 +1810,14 @@
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
+      <c r="Y30">
+        <v>26</v>
+      </c>
       <c r="Z30">
-        <v>26</v>
-      </c>
-      <c r="AA30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="10"/>
@@ -1768,9 +1836,8 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-    </row>
-    <row r="32" spans="1:27" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="10"/>
@@ -1789,9 +1856,8 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-    </row>
-    <row r="33" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="10"/>
@@ -1810,9 +1876,8 @@
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-    </row>
-    <row r="34" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="10"/>
@@ -1831,9 +1896,8 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-    </row>
-    <row r="35" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="10"/>
@@ -1852,9 +1916,8 @@
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-    </row>
-    <row r="36" spans="1:20" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:19" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1873,9 +1936,8 @@
       <c r="P36" s="8"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -1894,9 +1956,8 @@
       <c r="P37" s="8"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1915,9 +1976,8 @@
       <c r="P38" s="8"/>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1936,9 +1996,8 @@
       <c r="P39" s="8"/>
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1957,9 +2016,8 @@
       <c r="P40" s="8"/>
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1978,9 +2036,8 @@
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1999,9 +2056,8 @@
       <c r="P42" s="8"/>
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -2020,9 +2076,8 @@
       <c r="P43" s="8"/>
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -2041,7 +2096,6 @@
       <c r="P44" s="8"/>
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
-      <c r="S44" s="8"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_28 июня 2024 г. 22:18:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>Адеев Григорий</t>
   </si>
@@ -172,6 +172,21 @@
   </si>
   <si>
     <t xml:space="preserve">Л 3-4 </t>
+  </si>
+  <si>
+    <t>И 9</t>
+  </si>
+  <si>
+    <t>И 10</t>
+  </si>
+  <si>
+    <t>И 11</t>
+  </si>
+  <si>
+    <t>И 12</t>
+  </si>
+  <si>
+    <t>И 13</t>
   </si>
 </sst>
 </file>
@@ -588,13 +603,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFC44"/>
+  <dimension ref="A1:XFD44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -602,15 +617,19 @@
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
     <col min="2" max="2" width="21.453125" customWidth="1"/>
     <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="11" width="3" customWidth="1"/>
-    <col min="12" max="12" width="5.6328125" customWidth="1"/>
-    <col min="13" max="14" width="2.6328125" customWidth="1"/>
-    <col min="15" max="15" width="5.1796875" customWidth="1"/>
-    <col min="16" max="20" width="2.6328125" customWidth="1"/>
-    <col min="21" max="22" width="2.90625" customWidth="1"/>
+    <col min="4" max="10" width="3" customWidth="1"/>
+    <col min="11" max="11" width="2.81640625" customWidth="1"/>
+    <col min="12" max="12" width="2.81640625" style="6" customWidth="1"/>
+    <col min="13" max="16" width="3.1796875" customWidth="1"/>
+    <col min="17" max="17" width="5.1796875" customWidth="1"/>
+    <col min="18" max="19" width="2.6328125" customWidth="1"/>
+    <col min="20" max="20" width="6.6328125" customWidth="1"/>
+    <col min="21" max="21" width="2.6328125" customWidth="1"/>
+    <col min="22" max="25" width="2.90625" customWidth="1"/>
+    <col min="26" max="27" width="3.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26 16383:16383" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29 16384:16384" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
@@ -635,61 +654,76 @@
       <c r="K1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AC1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="XFC1" s="1"/>
-    </row>
-    <row r="2" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="XFD1" s="1"/>
+    </row>
+    <row r="2" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="Z2" s="15" t="s">
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="AC2" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f>IF(B3=C3,A2+1,"-----------------")</f>
         <v>1</v>
@@ -718,27 +752,27 @@
       <c r="J3" s="9">
         <v>5</v>
       </c>
-      <c r="M3" s="3">
-        <v>5</v>
-      </c>
-      <c r="N3" s="3">
-        <v>5</v>
-      </c>
-      <c r="O3" s="4">
-        <v>5</v>
-      </c>
-      <c r="P3" s="4">
-        <v>5</v>
-      </c>
-      <c r="S3" s="7"/>
-      <c r="Y3">
+      <c r="R3" s="3">
+        <v>5</v>
+      </c>
+      <c r="S3" s="3">
+        <v>5</v>
+      </c>
+      <c r="T3" s="4">
+        <v>5</v>
+      </c>
+      <c r="U3" s="4">
+        <v>5</v>
+      </c>
+      <c r="X3" s="7"/>
+      <c r="AB3">
         <v>11</v>
       </c>
-      <c r="Z3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A29" si="0">IF(B4=C4,A3+1,"-----------------")</f>
         <v>2</v>
@@ -751,31 +785,31 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="L4">
-        <v>5</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="P4">
-        <v>5</v>
-      </c>
       <c r="Q4">
         <v>5</v>
       </c>
-      <c r="R4" s="6">
-        <v>5</v>
-      </c>
-      <c r="S4">
-        <v>5</v>
-      </c>
-      <c r="Y4">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="U4">
+        <v>5</v>
+      </c>
+      <c r="V4">
+        <v>5</v>
+      </c>
+      <c r="W4" s="6">
+        <v>5</v>
+      </c>
+      <c r="X4">
+        <v>5</v>
+      </c>
+      <c r="AB4">
         <v>13</v>
       </c>
-      <c r="Z4">
+      <c r="AC4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -805,30 +839,30 @@
       <c r="K5" s="4">
         <v>5</v>
       </c>
-      <c r="L5" s="8">
-        <v>5</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="3">
-        <v>5</v>
-      </c>
-      <c r="P5" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q5">
-        <v>5</v>
-      </c>
-      <c r="R5" s="6">
-        <v>5</v>
-      </c>
-      <c r="Y5">
+      <c r="Q5" s="8">
+        <v>5</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="3">
+        <v>5</v>
+      </c>
+      <c r="U5" s="4">
+        <v>5</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+      <c r="W5" s="6">
+        <v>5</v>
+      </c>
+      <c r="AB5">
         <v>28</v>
       </c>
-      <c r="Z5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -841,17 +875,17 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="R6" s="6"/>
-      <c r="Y6">
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="W6" s="6"/>
+      <c r="AB6">
         <v>9</v>
       </c>
-      <c r="Z6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -868,25 +902,27 @@
       <c r="E7" s="3">
         <v>5</v>
       </c>
-      <c r="M7" s="3">
-        <v>5</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7">
-        <v>5</v>
-      </c>
-      <c r="Q7">
-        <v>5</v>
-      </c>
-      <c r="R7" s="6"/>
-      <c r="Y7">
+      <c r="R7" s="3">
+        <v>5</v>
+      </c>
+      <c r="S7" s="2">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="V7">
+        <v>5</v>
+      </c>
+      <c r="W7" s="6"/>
+      <c r="AB7">
         <v>14</v>
       </c>
-      <c r="Z7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -912,19 +948,19 @@
       <c r="J8" s="4">
         <v>5</v>
       </c>
-      <c r="M8" s="3">
-        <v>5</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="R8" s="6"/>
-      <c r="Y8">
+      <c r="R8" s="3">
+        <v>5</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="W8" s="6"/>
+      <c r="AB8">
         <v>1</v>
       </c>
-      <c r="Z8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -951,33 +987,33 @@
       <c r="J9" s="4">
         <v>5</v>
       </c>
-      <c r="L9" s="8">
-        <v>5</v>
-      </c>
-      <c r="M9" s="3">
-        <v>5</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="R9" s="6">
-        <v>5</v>
-      </c>
-      <c r="S9">
-        <v>5</v>
-      </c>
-      <c r="T9">
-        <v>5</v>
-      </c>
-      <c r="V9">
+      <c r="Q9" s="8">
+        <v>5</v>
+      </c>
+      <c r="R9" s="3">
+        <v>5</v>
+      </c>
+      <c r="S9" s="2"/>
+      <c r="W9" s="6">
+        <v>5</v>
+      </c>
+      <c r="X9">
         <v>5</v>
       </c>
       <c r="Y9">
+        <v>5</v>
+      </c>
+      <c r="AA9">
+        <v>5</v>
+      </c>
+      <c r="AB9">
         <v>10</v>
       </c>
-      <c r="Z9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1004,19 +1040,19 @@
       <c r="J10" s="4">
         <v>5</v>
       </c>
-      <c r="M10" s="3">
-        <v>5</v>
-      </c>
-      <c r="N10" s="2"/>
-      <c r="R10" s="6"/>
-      <c r="Y10">
+      <c r="R10" s="3">
+        <v>5</v>
+      </c>
+      <c r="S10" s="2"/>
+      <c r="W10" s="6"/>
+      <c r="AB10">
         <v>19</v>
       </c>
-      <c r="Z10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1031,19 +1067,19 @@
         <v>5</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="M11" s="3">
-        <v>5</v>
-      </c>
-      <c r="N11" s="2"/>
-      <c r="R11" s="6"/>
-      <c r="Y11">
+      <c r="R11" s="3">
+        <v>5</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="W11" s="6"/>
+      <c r="AB11">
         <v>8</v>
       </c>
-      <c r="Z11">
+      <c r="AC11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1066,21 +1102,21 @@
       <c r="G12" s="4">
         <v>5</v>
       </c>
-      <c r="M12" s="3">
-        <v>5</v>
-      </c>
-      <c r="N12" s="3">
-        <v>5</v>
-      </c>
-      <c r="R12" s="6"/>
-      <c r="Y12">
+      <c r="R12" s="3">
+        <v>5</v>
+      </c>
+      <c r="S12" s="3">
+        <v>5</v>
+      </c>
+      <c r="W12" s="6"/>
+      <c r="AB12">
         <v>20</v>
       </c>
-      <c r="Z12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1105,19 +1141,19 @@
       <c r="J13" s="8">
         <v>5</v>
       </c>
-      <c r="M13" s="3">
-        <v>5</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="R13" s="6"/>
-      <c r="Y13">
+      <c r="R13" s="3">
+        <v>5</v>
+      </c>
+      <c r="S13" s="2"/>
+      <c r="W13" s="6"/>
+      <c r="AB13">
         <v>25</v>
       </c>
-      <c r="Z13">
+      <c r="AC13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1130,14 +1166,14 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="R14" s="6"/>
-      <c r="Y14" s="6" t="s">
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="W14" s="6"/>
+      <c r="AB14" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1152,17 +1188,17 @@
         <v>5</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="R15" s="6"/>
-      <c r="Y15">
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="W15" s="6"/>
+      <c r="AB15">
         <v>16</v>
       </c>
-      <c r="Z15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26 16383:16383" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29 16384:16384" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1192,39 +1228,44 @@
       <c r="K16" s="4">
         <v>5</v>
       </c>
-      <c r="M16" s="3">
-        <v>5</v>
-      </c>
-      <c r="N16" s="2"/>
-      <c r="O16">
-        <v>5</v>
-      </c>
       <c r="P16">
         <v>5</v>
       </c>
-      <c r="Q16">
-        <v>5</v>
-      </c>
-      <c r="R16" s="6">
-        <v>5</v>
-      </c>
-      <c r="S16">
+      <c r="R16" s="3">
+        <v>5</v>
+      </c>
+      <c r="S16" s="2">
         <v>5</v>
       </c>
       <c r="T16">
         <v>5</v>
       </c>
+      <c r="U16">
+        <v>5</v>
+      </c>
       <c r="V16">
         <v>5</v>
       </c>
+      <c r="W16" s="6">
+        <v>5</v>
+      </c>
+      <c r="X16">
+        <v>5</v>
+      </c>
       <c r="Y16">
+        <v>5</v>
+      </c>
+      <c r="AA16">
+        <v>5</v>
+      </c>
+      <c r="AB16">
         <v>22</v>
       </c>
-      <c r="Z16">
+      <c r="AC16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1251,32 +1292,32 @@
       <c r="J17" s="4">
         <v>5</v>
       </c>
-      <c r="M17" s="3">
-        <v>5</v>
-      </c>
-      <c r="N17" s="3">
-        <v>5</v>
-      </c>
-      <c r="P17" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q17" s="12">
-        <v>5</v>
-      </c>
-      <c r="R17" s="6">
-        <v>5</v>
-      </c>
-      <c r="V17">
-        <v>5</v>
-      </c>
-      <c r="Y17">
+      <c r="R17" s="3">
+        <v>5</v>
+      </c>
+      <c r="S17" s="3">
+        <v>5</v>
+      </c>
+      <c r="U17" s="5">
+        <v>5</v>
+      </c>
+      <c r="V17" s="12">
+        <v>5</v>
+      </c>
+      <c r="W17" s="6">
+        <v>5</v>
+      </c>
+      <c r="AA17">
+        <v>5</v>
+      </c>
+      <c r="AB17">
         <v>9</v>
       </c>
-      <c r="Z17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1309,24 +1350,24 @@
       <c r="K18" s="4">
         <v>5</v>
       </c>
-      <c r="M18" s="3">
-        <v>5</v>
-      </c>
-      <c r="N18" s="3">
-        <v>5</v>
-      </c>
-      <c r="P18" s="4">
-        <v>5</v>
-      </c>
-      <c r="R18" s="6"/>
-      <c r="Y18">
+      <c r="R18" s="3">
+        <v>5</v>
+      </c>
+      <c r="S18" s="3">
+        <v>5</v>
+      </c>
+      <c r="U18" s="4">
+        <v>5</v>
+      </c>
+      <c r="W18" s="6"/>
+      <c r="AB18">
         <v>2</v>
       </c>
-      <c r="Z18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1344,19 +1385,19 @@
       <c r="F19" s="4">
         <v>5</v>
       </c>
-      <c r="M19" s="3">
-        <v>5</v>
-      </c>
-      <c r="N19" s="2"/>
-      <c r="R19" s="6"/>
-      <c r="Y19">
+      <c r="R19" s="3">
+        <v>5</v>
+      </c>
+      <c r="S19" s="2"/>
+      <c r="W19" s="6"/>
+      <c r="AB19">
         <v>17</v>
       </c>
-      <c r="Z19">
+      <c r="AC19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1386,24 +1427,24 @@
       <c r="K20" s="4">
         <v>5</v>
       </c>
-      <c r="L20">
-        <v>5</v>
-      </c>
-      <c r="M20" s="3">
-        <v>5</v>
-      </c>
-      <c r="N20" s="2">
-        <v>5</v>
-      </c>
-      <c r="P20" s="4">
-        <v>5</v>
-      </c>
-      <c r="R20" s="6"/>
-      <c r="Y20" t="s">
+      <c r="Q20">
+        <v>5</v>
+      </c>
+      <c r="R20" s="3">
+        <v>5</v>
+      </c>
+      <c r="S20" s="2">
+        <v>5</v>
+      </c>
+      <c r="U20" s="4">
+        <v>5</v>
+      </c>
+      <c r="W20" s="6"/>
+      <c r="AB20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1427,22 +1468,22 @@
       <c r="K21" s="4">
         <v>5</v>
       </c>
-      <c r="L21">
-        <v>5</v>
-      </c>
-      <c r="M21" s="3">
-        <v>5</v>
-      </c>
-      <c r="N21" s="2"/>
-      <c r="R21" s="6"/>
-      <c r="Y21">
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21" s="3">
+        <v>5</v>
+      </c>
+      <c r="S21" s="2"/>
+      <c r="W21" s="6"/>
+      <c r="AB21">
         <v>3</v>
       </c>
-      <c r="Z21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1457,21 +1498,21 @@
         <v>5</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="M22" s="3">
-        <v>5</v>
-      </c>
-      <c r="N22" s="3">
-        <v>5</v>
-      </c>
-      <c r="R22" s="6"/>
-      <c r="Y22">
+      <c r="R22" s="3">
+        <v>5</v>
+      </c>
+      <c r="S22" s="3">
+        <v>5</v>
+      </c>
+      <c r="W22" s="6"/>
+      <c r="AB22">
         <v>12</v>
       </c>
-      <c r="Z22">
+      <c r="AC22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1486,17 +1527,17 @@
         <v>5</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="R23" s="6"/>
-      <c r="Y23">
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="W23" s="6"/>
+      <c r="AB23">
         <v>21</v>
       </c>
-      <c r="Z23">
+      <c r="AC23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1520,30 +1561,32 @@
       <c r="J24">
         <v>5</v>
       </c>
-      <c r="M24" s="3">
-        <v>5</v>
-      </c>
-      <c r="N24" s="2"/>
-      <c r="O24">
-        <v>5</v>
-      </c>
-      <c r="P24">
-        <v>5</v>
-      </c>
-      <c r="Q24">
-        <v>5</v>
-      </c>
-      <c r="R24" s="6">
-        <v>5</v>
-      </c>
-      <c r="Y24">
+      <c r="R24" s="3">
+        <v>5</v>
+      </c>
+      <c r="S24" s="2">
+        <v>5</v>
+      </c>
+      <c r="T24">
+        <v>5</v>
+      </c>
+      <c r="U24">
+        <v>5</v>
+      </c>
+      <c r="V24">
+        <v>5</v>
+      </c>
+      <c r="W24" s="6">
+        <v>5</v>
+      </c>
+      <c r="AB24">
         <v>18</v>
       </c>
-      <c r="Z24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1578,38 +1621,38 @@
       <c r="K25" s="4">
         <v>5</v>
       </c>
-      <c r="L25" s="8">
-        <v>5</v>
-      </c>
-      <c r="M25" s="3">
-        <v>5</v>
-      </c>
-      <c r="N25" s="3">
-        <v>5</v>
-      </c>
-      <c r="P25" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q25">
-        <v>5</v>
-      </c>
-      <c r="R25" s="6">
-        <v>5</v>
-      </c>
-      <c r="S25">
-        <v>5</v>
-      </c>
-      <c r="T25">
+      <c r="Q25" s="8">
+        <v>5</v>
+      </c>
+      <c r="R25" s="3">
+        <v>5</v>
+      </c>
+      <c r="S25" s="3">
+        <v>5</v>
+      </c>
+      <c r="U25" s="4">
+        <v>5</v>
+      </c>
+      <c r="V25">
+        <v>5</v>
+      </c>
+      <c r="W25" s="6">
+        <v>5</v>
+      </c>
+      <c r="X25">
         <v>5</v>
       </c>
       <c r="Y25">
+        <v>5</v>
+      </c>
+      <c r="AB25">
         <v>27</v>
       </c>
-      <c r="Z25">
+      <c r="AC25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1644,23 +1687,10 @@
       <c r="K26" s="4">
         <v>5</v>
       </c>
-      <c r="M26" s="3">
-        <v>5</v>
-      </c>
-      <c r="N26" s="2"/>
-      <c r="O26">
-        <v>5</v>
-      </c>
-      <c r="P26">
-        <v>5</v>
-      </c>
-      <c r="Q26">
-        <v>5</v>
-      </c>
-      <c r="R26" s="6">
-        <v>5</v>
-      </c>
-      <c r="S26">
+      <c r="R26" s="3">
+        <v>5</v>
+      </c>
+      <c r="S26" s="2">
         <v>5</v>
       </c>
       <c r="T26">
@@ -1672,14 +1702,29 @@
       <c r="V26">
         <v>5</v>
       </c>
+      <c r="W26" s="6">
+        <v>5</v>
+      </c>
+      <c r="X26">
+        <v>5</v>
+      </c>
       <c r="Y26">
+        <v>5</v>
+      </c>
+      <c r="Z26">
+        <v>5</v>
+      </c>
+      <c r="AA26">
+        <v>5</v>
+      </c>
+      <c r="AB26">
         <v>22</v>
       </c>
-      <c r="Z26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1698,24 +1743,24 @@
       <c r="G27" s="4">
         <v>5</v>
       </c>
-      <c r="M27" s="3">
-        <v>5</v>
-      </c>
-      <c r="N27" s="3">
-        <v>5</v>
-      </c>
-      <c r="P27" s="4">
-        <v>5</v>
-      </c>
-      <c r="R27" s="6"/>
-      <c r="Y27">
+      <c r="R27" s="3">
+        <v>5</v>
+      </c>
+      <c r="S27" s="3">
+        <v>5</v>
+      </c>
+      <c r="U27" s="4">
+        <v>5</v>
+      </c>
+      <c r="W27" s="6"/>
+      <c r="AB27">
         <v>6</v>
       </c>
-      <c r="Z27">
+      <c r="AC27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1730,19 +1775,19 @@
         <v>5</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="M28" s="3">
-        <v>5</v>
-      </c>
-      <c r="N28" s="2"/>
-      <c r="R28" s="6"/>
-      <c r="Y28">
-        <v>5</v>
-      </c>
-      <c r="Z28">
+      <c r="R28" s="3">
+        <v>5</v>
+      </c>
+      <c r="S28" s="2"/>
+      <c r="W28" s="6"/>
+      <c r="AB28">
+        <v>5</v>
+      </c>
+      <c r="AC28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1774,22 +1819,22 @@
       <c r="K29" s="4">
         <v>5</v>
       </c>
-      <c r="M29" s="3">
-        <v>5</v>
-      </c>
-      <c r="N29" s="2"/>
-      <c r="Q29">
-        <v>5</v>
-      </c>
-      <c r="R29" s="6"/>
-      <c r="Y29">
+      <c r="R29" s="3">
+        <v>5</v>
+      </c>
+      <c r="S29" s="2"/>
+      <c r="V29">
+        <v>5</v>
+      </c>
+      <c r="W29" s="6"/>
+      <c r="AB29">
         <v>15</v>
       </c>
-      <c r="Z29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8" t="s">
         <v>31</v>
@@ -1803,21 +1848,21 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="Y30">
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="AB30">
         <v>26</v>
       </c>
-      <c r="Z30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="10"/>
@@ -1829,15 +1874,15 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-    </row>
-    <row r="32" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+    </row>
+    <row r="32" spans="1:29" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="10"/>
@@ -1849,15 +1894,15 @@
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-    </row>
-    <row r="33" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+    </row>
+    <row r="33" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="10"/>
@@ -1869,15 +1914,15 @@
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-    </row>
-    <row r="34" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+    </row>
+    <row r="34" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="10"/>
@@ -1889,15 +1934,15 @@
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-    </row>
-    <row r="35" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+    </row>
+    <row r="35" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="10"/>
@@ -1909,15 +1954,15 @@
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-    </row>
-    <row r="36" spans="1:19" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+    </row>
+    <row r="36" spans="1:24" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1929,15 +1974,15 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="8"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -1952,12 +1997,13 @@
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1972,12 +2018,13 @@
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1992,12 +2039,13 @@
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -2012,12 +2060,13 @@
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -2036,8 +2085,9 @@
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S41" s="8"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -2056,8 +2106,9 @@
       <c r="P42" s="8"/>
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S42" s="8"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -2076,8 +2127,9 @@
       <c r="P43" s="8"/>
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S43" s="8"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -2096,6 +2148,7 @@
       <c r="P44" s="8"/>
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_29 июня 2024 г. 0:02:50_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -609,7 +609,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -785,6 +785,12 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
       <c r="Q4">
         <v>5</v>
       </c>
@@ -902,6 +908,24 @@
       <c r="E7" s="3">
         <v>5</v>
       </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
       <c r="R7" s="3">
         <v>5</v>
       </c>
@@ -971,7 +995,9 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
       <c r="E9" s="3">
         <v>5</v>
       </c>
@@ -981,10 +1007,19 @@
       <c r="G9" s="4">
         <v>5</v>
       </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
       <c r="I9" s="4">
         <v>5</v>
       </c>
       <c r="J9" s="4">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="P9">
         <v>5</v>
       </c>
       <c r="Q9" s="8">
@@ -1209,7 +1244,9 @@
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
       <c r="E16" s="3">
         <v>5</v>
       </c>
@@ -1219,6 +1256,9 @@
       <c r="G16" s="4">
         <v>5</v>
       </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
       <c r="I16" s="4">
         <v>5</v>
       </c>
@@ -1226,6 +1266,15 @@
         <v>5</v>
       </c>
       <c r="K16" s="4">
+        <v>5</v>
+      </c>
+      <c r="L16" s="4">
+        <v>5</v>
+      </c>
+      <c r="M16" s="4">
+        <v>5</v>
+      </c>
+      <c r="N16" s="4">
         <v>5</v>
       </c>
       <c r="P16">
@@ -1561,6 +1610,9 @@
       <c r="J24">
         <v>5</v>
       </c>
+      <c r="K24">
+        <v>5</v>
+      </c>
       <c r="R24" s="3">
         <v>5</v>
       </c>
@@ -1621,6 +1673,12 @@
       <c r="K25" s="4">
         <v>5</v>
       </c>
+      <c r="N25" s="4">
+        <v>5</v>
+      </c>
+      <c r="O25">
+        <v>5</v>
+      </c>
       <c r="Q25" s="8">
         <v>5</v>
       </c>
@@ -1685,6 +1743,18 @@
         <v>5</v>
       </c>
       <c r="K26" s="4">
+        <v>5</v>
+      </c>
+      <c r="L26" s="4">
+        <v>5</v>
+      </c>
+      <c r="M26" s="4">
+        <v>5</v>
+      </c>
+      <c r="N26" s="4">
+        <v>5</v>
+      </c>
+      <c r="O26">
         <v>5</v>
       </c>
       <c r="R26" s="3">

</xml_diff>

<commit_message>
AutoCommit_11 июля 2024 г. 13:26:20_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -299,6 +299,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -609,7 +610,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -764,6 +765,12 @@
       <c r="U3" s="4">
         <v>5</v>
       </c>
+      <c r="V3">
+        <v>5</v>
+      </c>
+      <c r="W3">
+        <v>5</v>
+      </c>
       <c r="X3" s="7"/>
       <c r="AB3">
         <v>11</v>
@@ -938,7 +945,18 @@
       <c r="V7">
         <v>5</v>
       </c>
-      <c r="W7" s="6"/>
+      <c r="W7" s="6">
+        <v>5</v>
+      </c>
+      <c r="X7" s="16">
+        <v>5</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+      <c r="Z7">
+        <v>5</v>
+      </c>
       <c r="AB7">
         <v>14</v>
       </c>
@@ -1029,6 +1047,9 @@
         <v>5</v>
       </c>
       <c r="S9" s="2"/>
+      <c r="T9">
+        <v>5</v>
+      </c>
       <c r="W9" s="6">
         <v>5</v>
       </c>
@@ -1143,7 +1164,21 @@
       <c r="S12" s="3">
         <v>5</v>
       </c>
-      <c r="W12" s="6"/>
+      <c r="T12">
+        <v>5</v>
+      </c>
+      <c r="U12">
+        <v>5</v>
+      </c>
+      <c r="V12">
+        <v>5</v>
+      </c>
+      <c r="W12" s="6">
+        <v>5</v>
+      </c>
+      <c r="X12">
+        <v>5</v>
+      </c>
       <c r="AB12">
         <v>20</v>
       </c>
@@ -1180,6 +1215,9 @@
         <v>5</v>
       </c>
       <c r="S13" s="2"/>
+      <c r="T13">
+        <v>5</v>
+      </c>
       <c r="W13" s="6"/>
       <c r="AB13">
         <v>25</v>
@@ -1408,7 +1446,18 @@
       <c r="U18" s="4">
         <v>5</v>
       </c>
-      <c r="W18" s="6"/>
+      <c r="V18">
+        <v>5</v>
+      </c>
+      <c r="W18" s="6">
+        <v>5</v>
+      </c>
+      <c r="X18">
+        <v>5</v>
+      </c>
+      <c r="Y18">
+        <v>5</v>
+      </c>
       <c r="AB18">
         <v>2</v>
       </c>
@@ -1551,6 +1600,9 @@
         <v>5</v>
       </c>
       <c r="S22" s="3">
+        <v>5</v>
+      </c>
+      <c r="T22">
         <v>5</v>
       </c>
       <c r="W22" s="6"/>

</xml_diff>

<commit_message>
AutoCommit_11 июля 2024 г. 13:38:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -610,7 +610,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T23" sqref="T23"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -753,6 +753,9 @@
       <c r="J3" s="9">
         <v>5</v>
       </c>
+      <c r="K3" s="7">
+        <v>5</v>
+      </c>
       <c r="R3" s="3">
         <v>5</v>
       </c>
@@ -798,6 +801,9 @@
       <c r="N4">
         <v>5</v>
       </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
       <c r="Q4">
         <v>5</v>
       </c>
@@ -850,6 +856,12 @@
         <v>5</v>
       </c>
       <c r="K5" s="4">
+        <v>5</v>
+      </c>
+      <c r="L5" s="4">
+        <v>5</v>
+      </c>
+      <c r="N5" s="4">
         <v>5</v>
       </c>
       <c r="Q5" s="8">
@@ -1034,6 +1046,9 @@
       <c r="J9" s="4">
         <v>5</v>
       </c>
+      <c r="K9" s="7">
+        <v>5</v>
+      </c>
       <c r="M9">
         <v>5</v>
       </c>
@@ -1046,7 +1061,9 @@
       <c r="R9" s="3">
         <v>5</v>
       </c>
-      <c r="S9" s="2"/>
+      <c r="S9" s="2">
+        <v>5</v>
+      </c>
       <c r="T9">
         <v>5</v>
       </c>
@@ -1123,6 +1140,24 @@
         <v>5</v>
       </c>
       <c r="E11" s="2"/>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="4">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11" s="4">
+        <v>5</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
       <c r="R11" s="3">
         <v>5</v>
       </c>
@@ -1158,6 +1193,27 @@
       <c r="G12" s="4">
         <v>5</v>
       </c>
+      <c r="I12" s="4">
+        <v>5</v>
+      </c>
+      <c r="J12" s="4">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="L12" s="6">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
       <c r="R12" s="3">
         <v>5</v>
       </c>
@@ -1197,7 +1253,9 @@
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="4">
         <v>5</v>
@@ -1211,10 +1269,21 @@
       <c r="J13" s="8">
         <v>5</v>
       </c>
+      <c r="K13">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
       <c r="R13" s="3">
         <v>5</v>
       </c>
-      <c r="S13" s="2"/>
+      <c r="S13" s="2">
+        <v>5</v>
+      </c>
       <c r="T13">
         <v>5</v>
       </c>
@@ -1379,6 +1448,12 @@
       <c r="J17" s="4">
         <v>5</v>
       </c>
+      <c r="M17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
       <c r="R17" s="3">
         <v>5</v>
       </c>
@@ -1437,6 +1512,12 @@
       <c r="K18" s="4">
         <v>5</v>
       </c>
+      <c r="N18" s="4">
+        <v>5</v>
+      </c>
+      <c r="O18">
+        <v>5</v>
+      </c>
       <c r="R18" s="3">
         <v>5</v>
       </c>
@@ -1483,6 +1564,15 @@
       <c r="F19" s="4">
         <v>5</v>
       </c>
+      <c r="G19" s="4">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5</v>
+      </c>
       <c r="R19" s="3">
         <v>5</v>
       </c>
@@ -1596,6 +1686,24 @@
         <v>5</v>
       </c>
       <c r="E22" s="2"/>
+      <c r="F22" s="4">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22" s="4">
+        <v>5</v>
+      </c>
+      <c r="K22" s="4">
+        <v>5</v>
+      </c>
       <c r="R22" s="3">
         <v>5</v>
       </c>
@@ -1649,13 +1757,18 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
       <c r="E24" s="3">
         <v>5</v>
       </c>
       <c r="F24" s="4">
         <v>4</v>
       </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
       <c r="I24" s="4">
         <v>5</v>
       </c>
@@ -1663,6 +1776,18 @@
         <v>5</v>
       </c>
       <c r="K24">
+        <v>5</v>
+      </c>
+      <c r="L24" s="6">
+        <v>5</v>
+      </c>
+      <c r="M24">
+        <v>5</v>
+      </c>
+      <c r="N24">
+        <v>5</v>
+      </c>
+      <c r="O24">
         <v>5</v>
       </c>
       <c r="R24" s="3">
@@ -1809,6 +1934,9 @@
       <c r="O26">
         <v>5</v>
       </c>
+      <c r="P26" s="4">
+        <v>5</v>
+      </c>
       <c r="R26" s="3">
         <v>5</v>
       </c>
@@ -1939,6 +2067,12 @@
         <v>5</v>
       </c>
       <c r="K29" s="4">
+        <v>5</v>
+      </c>
+      <c r="L29" s="4">
+        <v>5</v>
+      </c>
+      <c r="N29" s="4">
         <v>5</v>
       </c>
       <c r="R29" s="3">

</xml_diff>

<commit_message>
AutoCommit_11 июля 2024 г. 14:04:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -610,7 +610,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -775,6 +775,15 @@
         <v>5</v>
       </c>
       <c r="X3" s="7"/>
+      <c r="Y3" s="7">
+        <v>5</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <v>5</v>
+      </c>
       <c r="AB3">
         <v>11</v>
       </c>
@@ -878,6 +887,12 @@
         <v>5</v>
       </c>
       <c r="W5" s="6">
+        <v>5</v>
+      </c>
+      <c r="X5" s="16">
+        <v>5</v>
+      </c>
+      <c r="Z5">
         <v>5</v>
       </c>
       <c r="AB5">
@@ -969,6 +984,9 @@
       <c r="Z7">
         <v>5</v>
       </c>
+      <c r="AA7">
+        <v>5</v>
+      </c>
       <c r="AB7">
         <v>14</v>
       </c>
@@ -1163,6 +1181,15 @@
       </c>
       <c r="S11" s="2"/>
       <c r="W11" s="6"/>
+      <c r="X11">
+        <v>5</v>
+      </c>
+      <c r="Y11">
+        <v>5</v>
+      </c>
+      <c r="Z11">
+        <v>5</v>
+      </c>
       <c r="AB11">
         <v>8</v>
       </c>
@@ -1288,6 +1315,9 @@
         <v>5</v>
       </c>
       <c r="W13" s="6"/>
+      <c r="X13">
+        <v>5</v>
+      </c>
       <c r="AB13">
         <v>25</v>
       </c>
@@ -1469,6 +1499,9 @@
       <c r="W17" s="6">
         <v>5</v>
       </c>
+      <c r="X17">
+        <v>5</v>
+      </c>
       <c r="AA17">
         <v>5</v>
       </c>
@@ -1714,6 +1747,15 @@
         <v>5</v>
       </c>
       <c r="W22" s="6"/>
+      <c r="X22">
+        <v>5</v>
+      </c>
+      <c r="Y22">
+        <v>5</v>
+      </c>
+      <c r="Z22">
+        <v>5</v>
+      </c>
       <c r="AB22">
         <v>12</v>
       </c>
@@ -1808,6 +1850,9 @@
       <c r="W24" s="6">
         <v>5</v>
       </c>
+      <c r="X24" s="16">
+        <v>5</v>
+      </c>
       <c r="AB24">
         <v>18</v>
       </c>
@@ -2083,6 +2128,9 @@
         <v>5</v>
       </c>
       <c r="W29" s="6"/>
+      <c r="X29">
+        <v>5</v>
+      </c>
       <c r="AB29">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_11 июля 2024 г. 15:12:12_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_ОпСис_.xlsx
@@ -610,7 +610,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
+      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -765,9 +765,7 @@
       <c r="T3" s="4">
         <v>5</v>
       </c>
-      <c r="U3" s="4">
-        <v>5</v>
-      </c>
+      <c r="U3" s="4"/>
       <c r="V3">
         <v>5</v>
       </c>
@@ -878,6 +876,9 @@
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="3">
+        <v>5</v>
+      </c>
+      <c r="T5">
         <v>5</v>
       </c>
       <c r="U5" s="4">
@@ -1085,6 +1086,12 @@
       <c r="T9">
         <v>5</v>
       </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
       <c r="W9" s="6">
         <v>5</v>
       </c>
@@ -1180,7 +1187,15 @@
         <v>5</v>
       </c>
       <c r="S11" s="2"/>
-      <c r="W11" s="6"/>
+      <c r="U11">
+        <v>5</v>
+      </c>
+      <c r="V11">
+        <v>5</v>
+      </c>
+      <c r="W11" s="6">
+        <v>5</v>
+      </c>
       <c r="X11">
         <v>5</v>
       </c>
@@ -1314,7 +1329,12 @@
       <c r="T13">
         <v>5</v>
       </c>
-      <c r="W13" s="6"/>
+      <c r="U13">
+        <v>5</v>
+      </c>
+      <c r="W13" s="6">
+        <v>5</v>
+      </c>
       <c r="X13">
         <v>5</v>
       </c>
@@ -1746,7 +1766,15 @@
       <c r="T22">
         <v>5</v>
       </c>
-      <c r="W22" s="6"/>
+      <c r="U22">
+        <v>5</v>
+      </c>
+      <c r="V22">
+        <v>5</v>
+      </c>
+      <c r="W22" s="6">
+        <v>5</v>
+      </c>
       <c r="X22">
         <v>5</v>
       </c>
@@ -2124,10 +2152,18 @@
         <v>5</v>
       </c>
       <c r="S29" s="2"/>
+      <c r="T29">
+        <v>5</v>
+      </c>
+      <c r="U29" s="4">
+        <v>5</v>
+      </c>
       <c r="V29">
         <v>5</v>
       </c>
-      <c r="W29" s="6"/>
+      <c r="W29" s="6">
+        <v>5</v>
+      </c>
       <c r="X29">
         <v>5</v>
       </c>

</xml_diff>